<commit_message>
1, 2, 3 calculations of Part 2
היא עוד לא הביאה חלק מהנתונים - אז שמתי ערך מדומה
ולכן אי אפשר להעריך אם התוצאות טובות כרגע
</commit_message>
<xml_diff>
--- a/data6.xlsx
+++ b/data6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tairhadad\Desktop\סמי שמעון\שנה ד\סמסטר ב\ישומי כלכלה\CompensationHW\CompensationHW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shir\Desktop\CompensationHW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334B5AFB-BCC6-40BF-B37E-F4D7C09EF947}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD60F8F-ABD4-464C-A25F-0CB722E2DB0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29295" yWindow="6255" windowWidth="14955" windowHeight="9375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43005" yWindow="0" windowWidth="14550" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$2:$P$152</definedName>
   </definedNames>
-  <calcPr calcId="181029" calcMode="autoNoTable"/>
+  <calcPr calcId="191029" calcMode="autoNoTable"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -887,32 +898,32 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="26">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="General_)"/>
-    <numFmt numFmtId="167" formatCode="#,###,###,###,###,###,###,###,###,###,###,###,###"/>
-    <numFmt numFmtId="168" formatCode="dd\-mmm\-yyyy"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00########"/>
-    <numFmt numFmtId="170" formatCode="#,##0.00%"/>
-    <numFmt numFmtId="171" formatCode="\+* #,##0.00;[Red]\-* #,##0.00"/>
-    <numFmt numFmtId="172" formatCode="\+* #,##0;[Red]\-* #,##0"/>
-    <numFmt numFmtId="173" formatCode="\ * #,##0;[Red]\-* #,##0"/>
-    <numFmt numFmtId="174" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
-    <numFmt numFmtId="175" formatCode="#.00"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00;\-* #,##0.00;_-* &quot;-&quot;??;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="#."/>
-    <numFmt numFmtId="178" formatCode="d\ mmmm\ yyyy"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00\ _B_F_-;\-* #,##0.00\ _B_F_-;_-* &quot;-&quot;??\ _B_F_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_ &quot;SFr.&quot;\ * #,##0_ ;_ &quot;SFr.&quot;\ * \-#,##0_ ;_ &quot;SFr.&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="_ &quot;SFr.&quot;\ * #,##0.00_ ;_ &quot;SFr.&quot;\ * \-#,##0.00_ ;_ &quot;SFr.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="182" formatCode="dd\ mmm\ yyyy"/>
-    <numFmt numFmtId="183" formatCode="###,###.##"/>
-    <numFmt numFmtId="184" formatCode="_-&quot;L.&quot;\ * #,##0_-;\-&quot;L.&quot;\ * #,##0_-;_-&quot;L.&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="185" formatCode="&quot;Fr.&quot;\+* #,##0.00;[Red]&quot;Fr.&quot;\-* #,##0.00"/>
-    <numFmt numFmtId="186" formatCode="&quot;Fr.&quot;\+* #,##0;[Red]&quot;Fr.&quot;\-* #,##0"/>
-    <numFmt numFmtId="187" formatCode="&quot;Fr.&quot;\ * #,##0;[Red]&quot;Fr.&quot;\-* #,##0"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="General_)"/>
+    <numFmt numFmtId="168" formatCode="#,###,###,###,###,###,###,###,###,###,###,###,###"/>
+    <numFmt numFmtId="169" formatCode="dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00########"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00%"/>
+    <numFmt numFmtId="172" formatCode="\+* #,##0.00;[Red]\-* #,##0.00"/>
+    <numFmt numFmtId="173" formatCode="\+* #,##0;[Red]\-* #,##0"/>
+    <numFmt numFmtId="174" formatCode="\ * #,##0;[Red]\-* #,##0"/>
+    <numFmt numFmtId="175" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
+    <numFmt numFmtId="176" formatCode="#.00"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00;\-* #,##0.00;_-* &quot;-&quot;??;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="#."/>
+    <numFmt numFmtId="179" formatCode="d\ mmmm\ yyyy"/>
+    <numFmt numFmtId="180" formatCode="_-* #,##0.00\ _B_F_-;\-* #,##0.00\ _B_F_-;_-* &quot;-&quot;??\ _B_F_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="_ &quot;SFr.&quot;\ * #,##0_ ;_ &quot;SFr.&quot;\ * \-#,##0_ ;_ &quot;SFr.&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="182" formatCode="_ &quot;SFr.&quot;\ * #,##0.00_ ;_ &quot;SFr.&quot;\ * \-#,##0.00_ ;_ &quot;SFr.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="183" formatCode="dd\ mmm\ yyyy"/>
+    <numFmt numFmtId="184" formatCode="###,###.##"/>
+    <numFmt numFmtId="185" formatCode="_-&quot;L.&quot;\ * #,##0_-;\-&quot;L.&quot;\ * #,##0_-;_-&quot;L.&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="186" formatCode="&quot;Fr.&quot;\+* #,##0.00;[Red]&quot;Fr.&quot;\-* #,##0.00"/>
+    <numFmt numFmtId="187" formatCode="&quot;Fr.&quot;\+* #,##0;[Red]&quot;Fr.&quot;\-* #,##0"/>
+    <numFmt numFmtId="188" formatCode="&quot;Fr.&quot;\ * #,##0;[Red]&quot;Fr.&quot;\-* #,##0"/>
   </numFmts>
   <fonts count="97">
     <font>
@@ -2395,8 +2406,8 @@
     <xf numFmtId="0" fontId="32" fillId="33" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="33" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="33" borderId="0"/>
-    <xf numFmtId="44" fontId="4" fillId="34" borderId="10"/>
-    <xf numFmtId="44" fontId="4" fillId="34" borderId="10"/>
+    <xf numFmtId="165" fontId="4" fillId="34" borderId="10"/>
+    <xf numFmtId="165" fontId="4" fillId="34" borderId="10"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
@@ -2518,7 +2529,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="79" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="38" fillId="48" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="80" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -2528,7 +2539,7 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="70" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="81" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="167" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="57" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2537,23 +2548,16 @@
     <xf numFmtId="0" fontId="35" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="67" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="77" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="77" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2575,13 +2579,20 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="1" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="42" fontId="4" fillId="71" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="71" borderId="0"/>
     <xf numFmtId="14" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="172" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="173" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="4" fillId="72" borderId="14"/>
+    <xf numFmtId="174" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="72" borderId="14"/>
     <xf numFmtId="0" fontId="43" fillId="73" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="74" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="75" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2593,17 +2604,17 @@
     <xf numFmtId="0" fontId="35" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="67" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="45" fillId="44" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="174" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="175" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="175" fontId="46" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="46" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="4" fillId="76" borderId="15"/>
+    <xf numFmtId="167" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="76" borderId="15"/>
     <xf numFmtId="49" fontId="25" fillId="77" borderId="15" applyFont="0"/>
     <xf numFmtId="0" fontId="83" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="48" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2628,10 +2639,10 @@
     <xf numFmtId="0" fontId="85" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="53" fillId="0" borderId="0">
+    <xf numFmtId="178" fontId="53" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="53" fillId="0" borderId="0">
+    <xf numFmtId="178" fontId="53" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2640,13 +2651,13 @@
     <xf numFmtId="0" fontId="54" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="87" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="55" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="55" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="180" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="181" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="89" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2670,7 +2681,7 @@
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="57" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -2834,7 +2845,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="182" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="183" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
@@ -2853,10 +2864,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="48" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="48" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="183" fontId="70" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="184" fontId="70" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2871,15 +2882,15 @@
     <xf numFmtId="0" fontId="73" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="183" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="184" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="54" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="184" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="185" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="186" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="187" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="188" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="58" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3712,8 +3723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:P152"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4222,7 +4233,7 @@
       <c r="O12" s="19"/>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1">
+    <row r="13" spans="1:16" ht="16.2" customHeight="1">
       <c r="A13" s="14">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -10236,7 +10247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>

</xml_diff>